<commit_message>
made a pdf and looked at the excel and
</commit_message>
<xml_diff>
--- a/14.04.2025 - Сравнительный анализ финансовых систем Китая, Индии с 15 другими странами БРИКС, АСЕАН и Запада/Тест Тьюки.xlsx
+++ b/14.04.2025 - Сравнительный анализ финансовых систем Китая, Индии с 15 другими странами БРИКС, АСЕАН и Запада/Тест Тьюки.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klyukin\Documents\Python Scripts\phd\conferences\14.04.2025 - Сравнительный анализ финансовых систем Китая, Индии с 15 другими странами БРИСК, АСЕАН и Запада\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Данные!$A$1:$J$1225</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
     <pivotCache cacheId="1" r:id="rId7"/>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="54">
   <si>
     <t>Factor</t>
   </si>
@@ -155,9 +150,6 @@
     <t>Сумма по полю 2 ^ meandiff</t>
   </si>
   <si>
-    <t>(несколько элементов)</t>
-  </si>
-  <si>
     <t>Normal 
 p -value level</t>
   </si>
@@ -189,14 +181,23 @@
   <si>
     <t>GREEN means we reject the null hypothesis and conclude that they are STATISTICALLY DIFFERENT and if RED - they are NOT statistically different.</t>
   </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -278,7 +279,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -289,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -299,7 +300,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="135" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -312,21 +313,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="77">
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
@@ -362,49 +363,49 @@
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
@@ -413,49 +414,49 @@
       <alignment textRotation="90" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
@@ -509,10 +510,10 @@
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
@@ -548,10 +549,10 @@
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _₽_-;\-* #,##0.000\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -27031,7 +27032,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Сумма по полю p-adj" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Сумма по полю p-adj" fld="4" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="13">
     <format dxfId="76">
@@ -28615,38 +28616,6 @@
     </format>
   </formats>
   <conditionalFormats count="2">
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="2" count="16">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-              <x v="10"/>
-              <x v="11"/>
-              <x v="12"/>
-              <x v="13"/>
-              <x v="14"/>
-              <x v="15"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
     <conditionalFormat priority="1">
       <pivotAreas count="15">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -28945,6 +28914,38 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="2" count="16">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
   </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -28956,7 +28957,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Сводная таблица1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Сводная таблица1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:Q20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -29128,7 +29129,7 @@
     <pageField fld="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Среднее по полю p-adj" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Среднее по полю p-adj" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="13">
     <format dxfId="0">
@@ -29238,9 +29239,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -29278,9 +29279,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -29315,7 +29316,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -29350,7 +29351,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -69990,7 +69991,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -70014,7 +70015,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -70044,7 +70045,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="62.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -75811,7 +75812,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -75832,7 +75833,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -76564,7 +76565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
@@ -76577,7 +76578,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -76598,7 +76599,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -81741,19 +81742,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="17" width="10.42578125" customWidth="1"/>
+    <col min="2" max="17" width="9.85546875" customWidth="1"/>
     <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -81762,7 +81763,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -81770,12 +81771,12 @@
         <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="62.25" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
@@ -82434,63 +82435,66 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>44</v>
-      </c>
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:17" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="14" t="s">
+    </row>
+    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
-        <f>(1/8)</f>
-        <v>0.125</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="15">
         <v>0.05</v>
       </c>
       <c r="D27" s="15">
-        <f>C27*A27</f>
+        <f>C27*A28</f>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <f>(1/8)</f>
+        <v>0.125</v>
+      </c>
       <c r="B28" s="13"/>
       <c r="C28" s="15">
         <v>0.1</v>
       </c>
       <c r="D28" s="15">
-        <f>C28*A27</f>
+        <f>C28*A28</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="4"/>
     </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="B5:Q20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="num" val="6.0000000000000001E-3"/>
-        <cfvo type="num" val="1.2999999999999999E-2"/>
-        <cfvo type="num" val="0.02"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="$D$27"/>
+        <cfvo type="num" val="$D$28"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>